<commit_message>
Happy Path Consulta y alta de controversias
</commit_message>
<xml_diff>
--- a/resources/InsumoControversias.xlsx
+++ b/resources/InsumoControversias.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\icf2303\Documents\Insumos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E262BB-FCDE-4EC5-A438-5D529CB6F6A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29D2067-DEA7-4B63-B10A-D6745D54EC15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8150" xr2:uid="{91FEA6BE-C469-4AAF-BB57-240240C8DE92}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="8150" activeTab="1" xr2:uid="{91FEA6BE-C469-4AAF-BB57-240240C8DE92}"/>
   </bookViews>
   <sheets>
-    <sheet name="Consulta Controversias" sheetId="1" r:id="rId1"/>
-    <sheet name="Alta Controversias" sheetId="2" r:id="rId2"/>
+    <sheet name="Consulta_Controversias" sheetId="1" r:id="rId1"/>
+    <sheet name="Alta_Controversias" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="49">
   <si>
     <t>BBVA perú</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Número de Cuenta</t>
   </si>
   <si>
-    <t>5204580000004121</t>
-  </si>
-  <si>
     <t>4551038224821285</t>
   </si>
   <si>
@@ -85,27 +82,15 @@
     <t>Afiliacion</t>
   </si>
   <si>
-    <t>Referencia</t>
-  </si>
-  <si>
     <t>Importe Facturación</t>
   </si>
   <si>
     <t>Número autorización</t>
   </si>
   <si>
-    <t>MasterCard</t>
-  </si>
-  <si>
     <t>BBVA Perú</t>
   </si>
   <si>
-    <t>20000158</t>
-  </si>
-  <si>
-    <t>20000161</t>
-  </si>
-  <si>
     <t>20230920</t>
   </si>
   <si>
@@ -121,78 +106,89 @@
     <t>066236</t>
   </si>
   <si>
-    <t>20230911</t>
-  </si>
-  <si>
-    <t>2223590100108114</t>
-  </si>
-  <si>
-    <t>744968</t>
-  </si>
-  <si>
-    <t>494362</t>
-  </si>
-  <si>
-    <t>440699</t>
-  </si>
-  <si>
     <t>72715813255100311300116</t>
   </si>
   <si>
-    <t>72715812195100102900061</t>
-  </si>
-  <si>
     <t>5124469999129999</t>
   </si>
   <si>
     <t>007176</t>
   </si>
   <si>
-    <t>4051420006041115</t>
-  </si>
-  <si>
     <t>902018</t>
   </si>
   <si>
-    <t>--</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	
-6401890045800006</t>
-  </si>
-  <si>
     <t>74745702010100101800235</t>
   </si>
   <si>
-    <t xml:space="preserve">	
-74745702166100309300105</t>
-  </si>
-  <si>
-    <t>4761140000000005</t>
-  </si>
-  <si>
-    <t>062748</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	
-74745703056100343800335</t>
-  </si>
-  <si>
     <t>Folio Controversias</t>
   </si>
   <si>
-    <t>062749</t>
-  </si>
-  <si>
-    <t>CC220616000001</t>
+    <t>CC220526000001</t>
+  </si>
+  <si>
+    <t>CC220616000015</t>
+  </si>
+  <si>
+    <t>6401890045800006</t>
+  </si>
+  <si>
+    <t>Moneda</t>
+  </si>
+  <si>
+    <t>Soles</t>
+  </si>
+  <si>
+    <t>Etapa</t>
+  </si>
+  <si>
+    <t>Solicitud de pagare</t>
+  </si>
+  <si>
+    <t>20231117</t>
+  </si>
+  <si>
+    <t>5115788000321431</t>
+  </si>
+  <si>
+    <t>175165</t>
+  </si>
+  <si>
+    <t>10006001</t>
+  </si>
+  <si>
+    <t>4919148000469196</t>
+  </si>
+  <si>
+    <t>175095</t>
+  </si>
+  <si>
+    <t>20231125</t>
+  </si>
+  <si>
+    <t>72715813329100311300134</t>
+  </si>
+  <si>
+    <t>20023320</t>
+  </si>
+  <si>
+    <t>653698</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -234,8 +230,6 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -243,6 +237,8 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,17 +553,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54CCEE73-2717-45BC-B929-602DECE7B477}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="20.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.36328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.6328125" bestFit="1" customWidth="1"/>
@@ -576,196 +572,199 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>20230823</v>
+      </c>
+      <c r="C2" s="2">
+        <v>20230823</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2">
+        <v>10003094</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="4">
+        <v>3325</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2">
+        <v>20230823</v>
+      </c>
+      <c r="C3" s="2">
+        <v>20230823</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="F3" s="2">
+        <v>10003094</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="4">
         <v>0</v>
       </c>
-      <c r="B2" s="4">
+      <c r="I3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2">
         <v>20230823</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C4" s="2">
         <v>20230823</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="D4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F4" s="2">
         <v>10003094</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="6">
+      <c r="G4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="4">
+        <v>3325</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="B5" s="2">
+        <v>20230823</v>
+      </c>
+      <c r="C5" s="2">
+        <v>20230823</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2">
+        <v>10003094</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="4">
         <v>0</v>
       </c>
-      <c r="B3" s="4">
-        <v>20231013</v>
-      </c>
-      <c r="C3" s="4">
-        <v>20231013</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="I5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2">
+        <v>20230823</v>
+      </c>
+      <c r="C6" s="2">
+        <v>20230823</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="4">
-        <v>20019348</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3" s="6">
-        <v>636.09</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="4">
-        <v>20230823</v>
-      </c>
-      <c r="C4" s="4">
-        <v>20230823</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="4">
+      <c r="F6" s="2">
         <v>10003094</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" s="6">
+      <c r="G6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="4">
         <v>3325</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="4">
-        <v>20230825</v>
-      </c>
-      <c r="C5" s="4">
-        <v>20230825</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="4">
-        <v>10006001</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H5" s="6">
-        <v>855.49</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="4">
-        <v>20230821</v>
-      </c>
-      <c r="C6" s="4">
-        <v>20231020</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="4">
-        <v>20019348</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="H6" s="6">
-        <v>100</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>50</v>
-      </c>
+      <c r="I6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G16" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -775,177 +774,254 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2BF3D99-C894-4F5F-A103-9735C80E97B0}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="4">
+        <v>24</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="4">
+        <v>85</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="4">
+        <v>18</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="C5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="F5" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="2">
-        <v>1</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="F6" s="4">
+        <v>21</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="2">
-        <v>400</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="H6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="4">
+        <v>85</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="2">
-        <v>640</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="2">
-        <v>3.5</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="2">
-        <v>21</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="F13" s="4">
+        <v>24</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F16" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Flujos Simples Controversias y Ventas
</commit_message>
<xml_diff>
--- a/resources/InsumoControversias.xlsx
+++ b/resources/InsumoControversias.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\icf2303\Documents\Insumos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29D2067-DEA7-4B63-B10A-D6745D54EC15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A4F893-F2C1-4B5D-9F98-26D5CC88E4DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="8150" activeTab="1" xr2:uid="{91FEA6BE-C469-4AAF-BB57-240240C8DE92}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="8150" xr2:uid="{91FEA6BE-C469-4AAF-BB57-240240C8DE92}"/>
   </bookViews>
   <sheets>
     <sheet name="Consulta_Controversias" sheetId="1" r:id="rId1"/>
-    <sheet name="Alta_Controversias" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId2"/>
+    <sheet name="Alta_Controversias" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="80">
   <si>
     <t>BBVA perú</t>
   </si>
@@ -124,12 +125,6 @@
     <t>Folio Controversias</t>
   </si>
   <si>
-    <t>CC220526000001</t>
-  </si>
-  <si>
-    <t>CC220616000015</t>
-  </si>
-  <si>
     <t>6401890045800006</t>
   </si>
   <si>
@@ -173,13 +168,112 @@
   </si>
   <si>
     <t>653698</t>
+  </si>
+  <si>
+    <t>Contracargo</t>
+  </si>
+  <si>
+    <t>Estatus</t>
+  </si>
+  <si>
+    <t>Cargo</t>
+  </si>
+  <si>
+    <t>Entregado</t>
+  </si>
+  <si>
+    <t>Pendiente automático</t>
+  </si>
+  <si>
+    <t>Pendiente de Cargo</t>
+  </si>
+  <si>
+    <t>Pendiente de recuperación</t>
+  </si>
+  <si>
+    <t>Rechazado</t>
+  </si>
+  <si>
+    <t>Recuperado</t>
+  </si>
+  <si>
+    <t>Representado</t>
+  </si>
+  <si>
+    <t>CC220619000006</t>
+  </si>
+  <si>
+    <t>CC220619000009</t>
+  </si>
+  <si>
+    <t>CC231108000009</t>
+  </si>
+  <si>
+    <t>CC220718000002</t>
+  </si>
+  <si>
+    <t>CC231114000007</t>
+  </si>
+  <si>
+    <t>CC220619000004</t>
+  </si>
+  <si>
+    <t>CC231027000003</t>
+  </si>
+  <si>
+    <t>902019</t>
+  </si>
+  <si>
+    <t>902020</t>
+  </si>
+  <si>
+    <t>902021</t>
+  </si>
+  <si>
+    <t>902022</t>
+  </si>
+  <si>
+    <t>902023</t>
+  </si>
+  <si>
+    <t>902024</t>
+  </si>
+  <si>
+    <t>902025</t>
+  </si>
+  <si>
+    <t>902026</t>
+  </si>
+  <si>
+    <t>SP231013000009</t>
+  </si>
+  <si>
+    <t>SP220620000001</t>
+  </si>
+  <si>
+    <t>SP220714000001</t>
+  </si>
+  <si>
+    <t>11111111111111</t>
+  </si>
+  <si>
+    <t>SP231206000008</t>
+  </si>
+  <si>
+    <t>SP230703000002</t>
+  </si>
+  <si>
+    <t>SP220626000020</t>
+  </si>
+  <si>
+    <t>SP231114000003</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,16 +281,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +301,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -228,17 +332,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,26 +660,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54CCEE73-2717-45BC-B929-602DECE7B477}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.90625" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" customWidth="1"/>
     <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.08984375" customWidth="1"/>
     <col min="9" max="9" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.54296875" customWidth="1"/>
+    <col min="11" max="11" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -599,172 +709,547 @@
       <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>20230823</v>
-      </c>
-      <c r="C2" s="2">
-        <v>20230823</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="K1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9">
+        <v>20230825</v>
+      </c>
+      <c r="C2" s="9">
+        <v>20230825</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="9">
         <v>10003094</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>3325</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="9">
+        <v>20230823</v>
+      </c>
+      <c r="C3" s="9">
+        <v>20230823</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="9">
+        <v>10003094</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="9">
+        <v>20230823</v>
+      </c>
+      <c r="C4" s="9">
+        <v>20230823</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2">
-        <v>20230823</v>
-      </c>
-      <c r="C3" s="2">
-        <v>20230823</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="9">
+        <v>10003094</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="3">
+        <v>3325</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="9">
+        <v>20230823</v>
+      </c>
+      <c r="C5" s="9">
+        <v>20230823</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="9">
+        <v>10003094</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="3">
+        <v>3325</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="9">
+        <v>20230822.199999999</v>
+      </c>
+      <c r="C6" s="9">
+        <v>20230823</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="9">
+        <v>10003094</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1995</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="9">
+        <v>20230821.800000001</v>
+      </c>
+      <c r="C7" s="9">
+        <v>20230823</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F7" s="9">
         <v>10003094</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="4">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3" t="s">
+      <c r="H7" s="3">
+        <v>1995</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2">
-        <v>20230823</v>
-      </c>
-      <c r="C4" s="2">
-        <v>20230823</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="J7" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="9">
+        <v>20230821.399999999</v>
+      </c>
+      <c r="C8" s="9">
+        <v>20230823</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F8" s="9">
         <v>10003094</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="4">
-        <v>3325</v>
-      </c>
-      <c r="I4" s="3" t="s">
+      <c r="H8" s="3">
+        <v>1995</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="9">
+        <v>20230821.399999999</v>
+      </c>
+      <c r="C9" s="9">
+        <v>20230823</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="2">
-        <v>20230823</v>
-      </c>
-      <c r="C5" s="2">
-        <v>20230823</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="2">
-        <v>10003094</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="4">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="2">
-        <v>20230823</v>
-      </c>
-      <c r="C6" s="2">
-        <v>20230823</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="2">
-        <v>10003094</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="F9" s="9">
+        <v>10003095</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="4">
-        <v>3325</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" s="3" t="s">
+      <c r="H9" s="3">
+        <v>1996</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="9">
+        <v>20230821.399999999</v>
+      </c>
+      <c r="C10" s="9">
+        <v>20230823</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="G16" s="6"/>
+      <c r="E10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="9">
+        <v>10003096</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1997</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="9">
+        <v>20230821.399999999</v>
+      </c>
+      <c r="C11" s="9">
+        <v>20230823</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="9">
+        <v>10003097</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1998</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="9">
+        <v>20230821.399999999</v>
+      </c>
+      <c r="C12" s="9">
+        <v>20230823</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="9">
+        <v>10003099</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="3">
+        <v>2000</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="9">
+        <v>20230821.399999999</v>
+      </c>
+      <c r="C13" s="9">
+        <v>20230823</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="9">
+        <v>10003100</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="3">
+        <v>2001</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="9">
+        <v>20230821.399999999</v>
+      </c>
+      <c r="C14" s="9">
+        <v>20230823</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="9">
+        <v>10003101</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="3">
+        <v>2002</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="9">
+        <v>20230821.399999999</v>
+      </c>
+      <c r="C15" s="9">
+        <v>20230823</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="9">
+        <v>10003102</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="3">
+        <v>2003</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -773,11 +1258,102 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34294F7D-9C10-45A2-A995-A323457D6001}">
+  <dimension ref="A2:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9">
+        <v>20230823</v>
+      </c>
+      <c r="C2" s="9">
+        <v>20230823</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="9">
+        <v>10003094</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="9">
+        <v>20230821.399999999</v>
+      </c>
+      <c r="C3" s="9">
+        <v>20230823</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="9">
+        <v>10003098</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1999</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2BF3D99-C894-4F5F-A103-9735C80E97B0}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -811,217 +1387,159 @@
         <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="C2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="3">
+        <v>24</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="3">
+        <v>85</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="3">
+        <v>18</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="H4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="4">
-        <v>24</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="F6" s="3">
+        <v>21</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="4">
-        <v>85</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="4">
-        <v>18</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="4">
-        <v>3.5</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="4">
-        <v>21</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="4">
-        <v>85</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="4">
-        <v>24</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="F16" s="7"/>
+      <c r="F13" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Comenzamos con nueva rama y todos los conflictos arreglados
</commit_message>
<xml_diff>
--- a/resources/InsumoControversias.xlsx
+++ b/resources/InsumoControversias.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\icf2303\Documents\Insumos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\icf2303\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A4F893-F2C1-4B5D-9F98-26D5CC88E4DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E94C92-A37B-4097-A7D0-75CB2FF49B7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="8150" xr2:uid="{91FEA6BE-C469-4AAF-BB57-240240C8DE92}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8150" xr2:uid="{91FEA6BE-C469-4AAF-BB57-240240C8DE92}"/>
   </bookViews>
   <sheets>
     <sheet name="Consulta_Controversias" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="3" r:id="rId2"/>
-    <sheet name="Alta_Controversias" sheetId="2" r:id="rId3"/>
+    <sheet name="Alta_Controversias" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1258,102 +1258,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34294F7D-9C10-45A2-A995-A323457D6001}">
-  <dimension ref="A2:L3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="9">
-        <v>20230823</v>
-      </c>
-      <c r="C2" s="9">
-        <v>20230823</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="9">
-        <v>10003094</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="9">
-        <v>20230821.399999999</v>
-      </c>
-      <c r="C3" s="9">
-        <v>20230823</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="9">
-        <v>10003098</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="3">
-        <v>1999</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2BF3D99-C894-4F5F-A103-9735C80E97B0}">
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1545,4 +1454,95 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34294F7D-9C10-45A2-A995-A323457D6001}">
+  <dimension ref="A2:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9">
+        <v>20230823</v>
+      </c>
+      <c r="C2" s="9">
+        <v>20230823</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="9">
+        <v>10003094</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="9">
+        <v>20230821.399999999</v>
+      </c>
+      <c r="C3" s="9">
+        <v>20230823</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="9">
+        <v>10003098</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1999</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>